<commit_message>
pre conversion to neondb
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>Transaction</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>maxSpend</t>
+  </si>
+  <si>
+    <t>Budgets</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -455,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>